<commit_message>
from SSL_CERTFICATE to NORMAL_CERTIFICATE
</commit_message>
<xml_diff>
--- a/licensedocs/certificate.xlsx
+++ b/licensedocs/certificate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ciradukunda/Documents/WORK/ElicenseUAT/license-management-system-frontend/licensedocs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23A96FCF-086B-9240-B71D-C27CAF192809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13B470C-EA0D-3243-B857-21EF4EAFA90B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18180" xr2:uid="{7914EAF3-C384-784C-8F99-7FBB6D8B84CB}"/>
   </bookViews>
@@ -62,12 +62,6 @@
     <t>DigiCert</t>
   </si>
   <si>
-    <t>Security certificate</t>
-  </si>
-  <si>
-    <t>RIPPS certificate</t>
-  </si>
-  <si>
     <t>RIPPS_CERTIFICATE</t>
   </si>
   <si>
@@ -75,6 +69,12 @@
   </si>
   <si>
     <t>expiration_date</t>
+  </si>
+  <si>
+    <t>Security certificatess</t>
+  </si>
+  <si>
+    <t>RIPPS certificatess</t>
   </si>
 </sst>
 </file>
@@ -453,7 +453,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -468,7 +468,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -477,7 +477,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -491,7 +491,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -514,7 +514,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -526,7 +526,7 @@
         <v>46219</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F3">
         <v>1</v>

</xml_diff>